<commit_message>
ADV APP IMP QUEUE feature
</commit_message>
<xml_diff>
--- a/queue-monitoring/src/main/resources/contracts/manual-contracts.xlsx
+++ b/queue-monitoring/src/main/resources/contracts/manual-contracts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="186">
   <si>
     <t>Customer</t>
   </si>
@@ -641,19 +641,25 @@
     <t>51434374/ 51394673</t>
   </si>
   <si>
-    <t>Sparda Datenverarbeitung</t>
-  </si>
-  <si>
     <t>Dnata</t>
   </si>
   <si>
-    <t>Avaya Agent for Desktop</t>
-  </si>
-  <si>
     <t>Apr, 1st 2016</t>
   </si>
   <si>
     <t>Mar, 30th 2019</t>
+  </si>
+  <si>
+    <t>Avaya Agent for Desktop, Survey Assist, CBA and Dynamic Routing</t>
+  </si>
+  <si>
+    <t>Sparda Datenverarbeitung - I14DE1920 (Phase 1) and I15DE1953 (Phase 2)</t>
+  </si>
+  <si>
+    <t>ATLAS Contract</t>
+  </si>
+  <si>
+    <t>AIC AAWC</t>
   </si>
 </sst>
 </file>
@@ -2347,10 +2353,10 @@
         <v>31</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="13" t="s">
@@ -3024,42 +3030,69 @@
       <c r="I71" s="15"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B72" s="6">
-        <v>50244545</v>
-      </c>
-      <c r="C72" s="10"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="D72" s="5"/>
       <c r="E72" s="12"/>
       <c r="F72" s="8"/>
       <c r="G72" s="8"/>
-      <c r="H72" s="3"/>
+      <c r="H72" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="I72" s="15"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B73" s="6"/>
-      <c r="C73" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="D73" s="5"/>
-      <c r="E73" s="12"/>
+        <v>183</v>
+      </c>
+      <c r="B73" s="6">
+        <v>50244545</v>
+      </c>
+      <c r="C73" s="10"/>
+      <c r="D73" s="5">
+        <v>198427</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
       <c r="H73" s="4" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="I73" s="15"/>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="17"/>
+    <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" s="6">
+        <v>50244545</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D74" s="5">
+        <v>198429</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F74" s="8"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I74" s="15"/>
+      <c r="J74" s="3"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B75" s="17"/>
@@ -3069,9 +3102,6 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" s="17"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="17"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81"/>

</xml_diff>

<commit_message>
Adjustments related to the new Duty Shift Process.
</commit_message>
<xml_diff>
--- a/queue-monitoring/src/main/resources/contracts/manual-contracts.xlsx
+++ b/queue-monitoring/src/main/resources/contracts/manual-contracts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="209">
   <si>
     <t>Customer</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Link to SAP Documentation</t>
-  </si>
-  <si>
-    <t>Comments to Apps Supp Team</t>
   </si>
   <si>
     <t>Telcel (Venezuela)</t>
@@ -656,10 +653,82 @@
     <t>Sparda Datenverarbeitung - I14DE1920 (Phase 1) and I15DE1953 (Phase 2)</t>
   </si>
   <si>
-    <t>ATLAS Contract</t>
-  </si>
-  <si>
-    <t>AIC AAWC</t>
+    <t>Comments to Apps Supp Team / KT</t>
+  </si>
+  <si>
+    <t>US / EMEA</t>
+  </si>
+  <si>
+    <t>NLP language detection Snap-in</t>
+  </si>
+  <si>
+    <t>\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Tesla Motors\SOW\Manual Contract</t>
+  </si>
+  <si>
+    <t>https://confluence.forge.avaya.com/display/EPTADVANCEDAPPS/Tesla+Motors#TeslaMotors-Forge/ConfluenceDetail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Call Management System External Call History Handler for Operational Analyst </t>
+  </si>
+  <si>
+    <t>ATLAS Contract (Germany)</t>
+  </si>
+  <si>
+    <t>\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Sparda\SOW\Manual Contract</t>
+  </si>
+  <si>
+    <t>Interaction Center/Operational Analyst - Customized AAWC with screen pop up</t>
+  </si>
+  <si>
+    <t>Supported by Midiavox - https://confluence.forge.avaya.com/display/EPTADVANCEDAPPS/Sparda+Datenverarbeitung</t>
+  </si>
+  <si>
+    <t>AOK</t>
+  </si>
+  <si>
+    <t>Supported by Optisoft - Software Reselling</t>
+  </si>
+  <si>
+    <t>Mellitta</t>
+  </si>
+  <si>
+    <t>\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Melitta Professional Coffee Solutions\SOW\Manual Contract</t>
+  </si>
+  <si>
+    <t>Transgourmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREFISA SA CREDITO FINANCIAMENTO E </t>
+  </si>
+  <si>
+    <t>INTELLIGENT CALLBACK</t>
+  </si>
+  <si>
+    <t>Supported by Midiavox</t>
+  </si>
+  <si>
+    <t>AUSTIN ENERGY</t>
+  </si>
+  <si>
+    <t>Custom IVR Application</t>
+  </si>
+  <si>
+    <t>\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Austin Energy\SOW\Manual Contract</t>
+  </si>
+  <si>
+    <t>Supported by Servion</t>
+  </si>
+  <si>
+    <t>PETROBRAS DISTRIBUIDORA</t>
+  </si>
+  <si>
+    <t>CMS CUSTOM REPORT / CMS REMOTE C-LAN AND PBX LINK ADMINISTRATION/ CMS WFM REAL TIME / CMS WFM ADD ACD/SESSION/CONNECTION / CMS WFM HISTORICAL / CMS WFM ADD ACD HISTORICAL / IVR</t>
+  </si>
+  <si>
+    <t>CUSTOM IVR</t>
+  </si>
+  <si>
+    <t>CUSTOM IC TOOLBAR</t>
   </si>
 </sst>
 </file>
@@ -763,7 +832,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -805,15 +874,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1116,24 +1186,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J81"/>
+  <dimension ref="A2:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="C69" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" style="18" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="17" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.42578125" style="18" customWidth="1"/>
-    <col min="10" max="10" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.42578125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="38.28515625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1165,976 +1235,976 @@
         <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>9</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="5">
         <v>198427</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="5">
         <v>198431</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5">
         <v>198427</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="3"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5">
         <v>198427</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="3"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5">
         <v>198427</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5">
         <v>198427</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5">
         <v>198431</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="5">
         <v>198429</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D12" s="5">
         <v>198431</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="5">
         <v>198427</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5">
         <v>198427</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="3"/>
+      <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="5">
         <v>198427</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="5">
         <v>198427</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5">
         <v>198431</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="3"/>
+      <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5">
         <v>198429</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="3"/>
+      <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="D19" s="5">
         <v>198433</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="3"/>
+      <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="4"/>
       <c r="F20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="3"/>
+      <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="5">
         <v>198429</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="6">
         <v>50282971</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5">
         <v>198433</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="3"/>
+      <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="6">
         <v>50247790</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="5">
         <v>198433</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="3"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="6">
         <v>50247790</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="5">
         <v>198431</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="3"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="D25" s="5">
         <v>198433</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D26" s="5">
         <v>198427</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="4"/>
-      <c r="J26" s="3"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D27" s="5">
         <v>198429</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="3"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="D28" s="5">
         <v>198429</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="3"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="6">
         <v>50201622</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="5">
         <v>198429</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="3"/>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D30" s="5">
         <v>198429</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="I30" s="4"/>
-      <c r="J30" s="3"/>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D31" s="5">
         <v>198433</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="I31" s="4"/>
-      <c r="J31" s="3"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="D32" s="5">
         <v>198427</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="I32" s="4"/>
-      <c r="J32" s="3"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="6">
         <v>50537249</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="5">
         <v>198427</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F33" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="3"/>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="6">
         <v>50258996</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="5">
         <v>198429</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="3"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="6">
         <v>50933137</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="5">
         <v>198427</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F35" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="6">
         <v>50933137</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D36" s="5">
         <v>198429</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="4"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="D37" s="5">
         <v>198427</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F37" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>89</v>
-      </c>
       <c r="C38" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="5">
         <v>198429</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F38" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39" s="6">
         <v>50454348</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D39" s="5">
         <v>198427</v>
       </c>
       <c r="E39" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="D40" s="5">
         <v>198433</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F40" s="8">
         <v>41913</v>
@@ -2143,26 +2213,26 @@
         <v>43100</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I40" s="4"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D41" s="5">
         <v>198433</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F41" s="8">
         <v>41913</v>
@@ -2171,26 +2241,26 @@
         <v>43100</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" s="5">
         <v>198427</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42" s="8">
         <v>41913</v>
@@ -2199,26 +2269,26 @@
         <v>43100</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="J42" s="3"/>
+      <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D43" s="5">
         <v>198429</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F43" s="8">
         <v>41913</v>
@@ -2227,26 +2297,26 @@
         <v>43100</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D44" s="5">
         <v>198433</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F44" s="8">
         <v>41913</v>
@@ -2255,274 +2325,276 @@
         <v>43100</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="5">
+        <v>198433</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="8">
+        <v>41913</v>
+      </c>
+      <c r="G45" s="8">
+        <v>43100</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I45" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="4" t="s">
+      <c r="D46" s="5">
+        <v>198429</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D45" s="5">
-        <v>198429</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="G46" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="H46" s="3"/>
+      <c r="I46" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H45" s="3"/>
-      <c r="I45" s="4" t="s">
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="B47" s="6">
+        <v>50529465</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="6">
-        <v>50529465</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="5">
+      <c r="D47" s="5">
         <v>198427</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F46" s="8">
+      <c r="E47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="8">
         <v>42094</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G47" s="8">
         <v>43192</v>
-      </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="6">
-        <v>50396054</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="H47" s="3"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="6">
+        <v>50396054</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="1:10" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="C49" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="D49" s="11">
+        <v>198433</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="H49" s="7"/>
+      <c r="I49" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D48" s="11">
-        <v>198433</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="H48" s="7"/>
-      <c r="I48" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B49" s="6">
-        <v>50497974</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D49" s="5">
-        <v>198429</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="G49" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="J49" s="3"/>
+      <c r="J49" s="12"/>
     </row>
     <row r="50" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B50" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="B50" s="6">
+        <v>50497974</v>
+      </c>
       <c r="C50" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D50" s="11">
-        <v>198433</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>31</v>
+        <v>121</v>
+      </c>
+      <c r="D50" s="5">
+        <v>198429</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I50" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="J50" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="I50" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J50" s="4"/>
     </row>
     <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D51" s="5">
+        <v>126</v>
+      </c>
+      <c r="D51" s="11">
+        <v>198433</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D52" s="5">
         <v>198427</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F51" s="8" t="s">
+      <c r="E52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G52" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="H52" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="I52" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="I51" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="11">
-        <v>198433</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I52" s="16"/>
-      <c r="J52" s="3"/>
+      <c r="J52" s="4"/>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
+      </c>
+      <c r="D53" s="11">
+        <v>198433</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F53" s="8">
-        <v>42614</v>
-      </c>
-      <c r="G53" s="8">
-        <v>42979</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I53" s="4"/>
-      <c r="J53" s="3" t="s">
-        <v>157</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I53" s="16"/>
+      <c r="J53" s="4"/>
     </row>
     <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="B54" s="6" t="s">
-        <v>165</v>
-      </c>
       <c r="C54" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F54" s="8">
         <v>42614</v>
@@ -2531,28 +2603,28 @@
         <v>42979</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I54" s="4"/>
-      <c r="J54" s="3" t="s">
-        <v>157</v>
+      <c r="J54" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C55" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F55" s="8">
         <v>42614</v>
@@ -2561,28 +2633,28 @@
         <v>42979</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I55" s="4"/>
-      <c r="J55" s="3" t="s">
-        <v>157</v>
+      <c r="J55" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C56" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F56" s="8">
         <v>42614</v>
@@ -2591,28 +2663,28 @@
         <v>42979</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I56" s="4"/>
-      <c r="J56" s="3" t="s">
-        <v>157</v>
+      <c r="J56" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C57" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F57" s="8">
         <v>42614</v>
@@ -2621,28 +2693,28 @@
         <v>42979</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I57" s="4"/>
-      <c r="J57" s="3" t="s">
-        <v>157</v>
+      <c r="J57" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C58" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="E58" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F58" s="8">
         <v>42614</v>
@@ -2651,28 +2723,28 @@
         <v>42979</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I58" s="4"/>
-      <c r="J58" s="3" t="s">
-        <v>157</v>
+      <c r="J58" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C59" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="E59" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F59" s="8">
         <v>42614</v>
@@ -2681,28 +2753,28 @@
         <v>42979</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I59" s="4"/>
-      <c r="J59" s="3" t="s">
-        <v>157</v>
+      <c r="J59" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C60" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="E60" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F60" s="8">
         <v>42614</v>
@@ -2711,28 +2783,28 @@
         <v>42979</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I60" s="4"/>
-      <c r="J60" s="3" t="s">
-        <v>157</v>
+      <c r="J60" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C61" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="E61" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F61" s="8">
         <v>42614</v>
@@ -2741,58 +2813,58 @@
         <v>42979</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I61" s="4"/>
-      <c r="J61" s="3" t="s">
-        <v>157</v>
+      <c r="J61" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F62" s="8">
+        <v>42614</v>
+      </c>
+      <c r="G62" s="8">
+        <v>42979</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C63" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="D62" s="5">
+      <c r="D63" s="5">
         <v>198427</v>
       </c>
-      <c r="E62" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F62" s="8">
-        <v>42822</v>
-      </c>
-      <c r="G62" s="8">
-        <v>43186</v>
-      </c>
-      <c r="H62" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I62" s="4"/>
-      <c r="J62" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="D63" s="5">
-        <v>198429</v>
-      </c>
       <c r="E63" s="12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F63" s="8">
         <v>42822</v>
@@ -2801,56 +2873,58 @@
         <v>43186</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I63" s="4"/>
-      <c r="J63" s="3" t="s">
-        <v>176</v>
+      <c r="J63" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C64" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D64" s="5">
+        <v>198429</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="8">
+        <v>42822</v>
+      </c>
+      <c r="G64" s="8">
+        <v>43186</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="E65" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="F64" s="8">
-        <v>42614</v>
-      </c>
-      <c r="G64" s="8">
-        <v>42979</v>
-      </c>
-      <c r="H64" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="I64" s="4"/>
-      <c r="J64" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B65" s="6"/>
-      <c r="C65" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="5">
-        <v>198429</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="F65" s="8">
         <v>42614</v>
@@ -2858,83 +2932,83 @@
       <c r="G65" s="8">
         <v>42979</v>
       </c>
-      <c r="H65" s="3" t="s">
-        <v>75</v>
+      <c r="H65" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="I65" s="4"/>
-      <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="J65" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B66" s="6"/>
       <c r="C66" s="10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D66" s="5">
-        <v>198433</v>
+        <v>198429</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F66" s="8">
-        <v>42663</v>
+        <v>42614</v>
       </c>
       <c r="G66" s="8">
-        <v>43027</v>
-      </c>
-      <c r="H66" s="3"/>
-      <c r="I66" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>146</v>
-      </c>
+        <v>42979</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
     </row>
     <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B67" s="6">
-        <v>51319370</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="B67" s="6"/>
       <c r="C67" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D67" s="5">
-        <v>198427</v>
+        <v>198433</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F67" s="8">
-        <v>42719</v>
+        <v>42663</v>
       </c>
       <c r="G67" s="8">
-        <v>43083</v>
-      </c>
-      <c r="H67" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I67" s="4"/>
-      <c r="J67" s="3"/>
+        <v>43027</v>
+      </c>
+      <c r="H67" s="3"/>
+      <c r="I67" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
+      </c>
+      <c r="B68" s="6">
+        <v>51319370</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D68" s="5">
         <v>198427</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F68" s="8">
         <v>42719</v>
@@ -2943,183 +3017,411 @@
         <v>43083</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I68" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="J68" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
     </row>
     <row r="69" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="5">
+        <v>198427</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="8">
+        <v>42719</v>
+      </c>
+      <c r="G69" s="8">
+        <v>43083</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I69" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="J69" s="4"/>
+    </row>
+    <row r="70" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="6">
+        <v>50272257</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B69" s="6">
-        <v>50272257</v>
-      </c>
-      <c r="C69" s="10" t="s">
+      <c r="D70" s="5"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="8">
+        <v>42736</v>
+      </c>
+      <c r="G70" s="8">
+        <v>43100</v>
+      </c>
+      <c r="H70" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D69" s="5"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="8">
-        <v>42736</v>
-      </c>
-      <c r="G69" s="8">
-        <v>43100</v>
-      </c>
-      <c r="H69" s="3" t="s">
+      <c r="I70" s="15"/>
+      <c r="J70" s="4"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="I69" s="15"/>
-      <c r="J69" s="3"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B70" s="6">
+      <c r="B71" s="6">
         <v>5238072</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D70" s="5">
+      <c r="C71" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="5">
         <v>198433</v>
       </c>
-      <c r="E70" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F70" s="8">
+      <c r="E71" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" s="8">
         <v>42767</v>
       </c>
-      <c r="G70" s="8">
+      <c r="G71" s="8">
         <v>43131</v>
       </c>
-      <c r="H70" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I70" s="15"/>
-      <c r="J70" s="3"/>
-    </row>
-    <row r="71" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="H71" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I71" s="15"/>
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B72" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="C72" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D71" s="5">
+      <c r="D72" s="5">
         <v>198427</v>
       </c>
-      <c r="E71" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F71" s="8">
+      <c r="E72" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="8">
         <v>42084</v>
       </c>
-      <c r="G71" s="8">
+      <c r="G72" s="8">
         <v>43179</v>
       </c>
-      <c r="H71" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I71" s="15"/>
-      <c r="J71" s="3"/>
-    </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B72" s="6"/>
-      <c r="C72" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="D72" s="5"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="4" t="s">
-        <v>164</v>
+      <c r="H72" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="I72" s="15"/>
-      <c r="J72" s="3"/>
+      <c r="J72" s="4"/>
     </row>
     <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="B73" s="6">
-        <v>50244545</v>
-      </c>
-      <c r="C73" s="10"/>
-      <c r="D73" s="5">
-        <v>198427</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>13</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="5"/>
+      <c r="E73" s="12"/>
       <c r="F73" s="8"/>
       <c r="G73" s="8"/>
       <c r="H73" s="4" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="I73" s="15"/>
-      <c r="J73" s="3"/>
+      <c r="J73" s="4"/>
     </row>
     <row r="74" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B74" s="6">
         <v>50244545</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D74" s="5">
-        <v>198429</v>
+        <v>198427</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F74" s="8"/>
       <c r="G74" s="8"/>
       <c r="H74" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="I74" s="15"/>
-      <c r="J74" s="3"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="17"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="17"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="17"/>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81"/>
-      <c r="C81"/>
-      <c r="D81"/>
-      <c r="E81"/>
-      <c r="I81"/>
+        <v>189</v>
+      </c>
+      <c r="I74" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" s="6">
+        <v>50244545</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D75" s="5">
+        <v>198429</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F75" s="8"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I75" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I76" s="15"/>
+      <c r="J76" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77" s="6">
+        <v>51541248</v>
+      </c>
+      <c r="C77" s="10"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="8">
+        <v>42644</v>
+      </c>
+      <c r="G77" s="8">
+        <v>43373</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I77" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="8"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I78" s="15"/>
+      <c r="J78" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79" s="6">
+        <v>50428443</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="D79" s="5">
+        <v>198433</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F79" s="8">
+        <v>43159</v>
+      </c>
+      <c r="G79" s="8">
+        <v>43251</v>
+      </c>
+      <c r="H79" s="4"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D80" s="5">
+        <v>198433</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F80" s="8">
+        <v>42880</v>
+      </c>
+      <c r="G80" s="8">
+        <v>43244</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I80" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B81" s="6">
+        <v>50488074</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="5">
+        <v>198427</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="8">
+        <v>42217</v>
+      </c>
+      <c r="G81" s="8">
+        <v>43373</v>
+      </c>
+      <c r="H81" s="3"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="4"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B82" s="6">
+        <v>50488074</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D82" s="5">
+        <v>198433</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F82" s="8">
+        <v>42217</v>
+      </c>
+      <c r="G82" s="8">
+        <v>43373</v>
+      </c>
+      <c r="H82" s="3"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" s="6">
+        <v>50488074</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D83" s="5">
+        <v>198429</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F83" s="8">
+        <v>42217</v>
+      </c>
+      <c r="G83" s="8">
+        <v>43373</v>
+      </c>
+      <c r="H83" s="3"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="4" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B26" r:id="rId1" display="http://report.avaya.com/siebelreports/fldrill.aspx?site_id=0050221401"/>
-    <hyperlink ref="I45" r:id="rId2" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\PT"/>
-    <hyperlink ref="I49" r:id="rId3" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\PRUDENTIAL"/>
-    <hyperlink ref="I50" r:id="rId4" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Tongyang_TAK_POM\Manual"/>
-    <hyperlink ref="I51" r:id="rId5" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Tongyang_TAK_POM\Manual"/>
-    <hyperlink ref="I66" r:id="rId6" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Atio"/>
-    <hyperlink ref="I48" r:id="rId7"/>
-    <hyperlink ref="I68" r:id="rId8" location=" I17ID1004)\SOW\Manual Contract"/>
+    <hyperlink ref="I46" r:id="rId2" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\PT"/>
+    <hyperlink ref="I50" r:id="rId3" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\PRUDENTIAL"/>
+    <hyperlink ref="I51" r:id="rId4" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Tongyang_TAK_POM\Manual"/>
+    <hyperlink ref="I52" r:id="rId5" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Tongyang_TAK_POM\Manual"/>
+    <hyperlink ref="I67" r:id="rId6" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Atio"/>
+    <hyperlink ref="I49" r:id="rId7"/>
+    <hyperlink ref="I69" r:id="rId8" location=" I17ID1004)\SOW\Manual Contract"/>
+    <hyperlink ref="J45" r:id="rId9" location="TeslaMotors-Forge/ConfluenceDetail" display="https://confluence.forge.avaya.com/display/EPTADVANCEDAPPS/Tesla+Motors - TeslaMotors-Forge/ConfluenceDetail"/>
+    <hyperlink ref="I74" r:id="rId10" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Sparda\SOW\Manual"/>
+    <hyperlink ref="I75" r:id="rId11" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Sparda\SOW\Manual"/>
+    <hyperlink ref="I45" r:id="rId12" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Tesla"/>
+    <hyperlink ref="I77" r:id="rId13" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Melitta"/>
+    <hyperlink ref="I80" r:id="rId14" display="\\wmnas1.dr.avaya.com\customapplicationsupport\Accounts\Austin"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>